<commit_message>
clarifying roles for 2021
</commit_message>
<xml_diff>
--- a/Policies/PoliciesFiles/2020vs2019AttandanceComparision.xlsx
+++ b/Policies/PoliciesFiles/2020vs2019AttandanceComparision.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mashka/Desktop/Data Scientista/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jayspain/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A60C0FD7-28C7-1C45-B415-33AD936B7D8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA0AC67A-AF4B-5747-9466-81C743AE7310}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16000" xr2:uid="{31C23D92-A3D2-484D-839D-CEC35D2EDDC1}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16000" activeTab="2" xr2:uid="{31C23D92-A3D2-484D-839D-CEC35D2EDDC1}"/>
   </bookViews>
   <sheets>
     <sheet name="2019 vs 2020" sheetId="3" r:id="rId1"/>
@@ -18,9 +18,10 @@
     <sheet name="2020" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2019'!$A$1:$Z$84</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2020'!$C$1:$C$115</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1579" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1598" uniqueCount="390">
   <si>
     <t>Yes</t>
   </si>
@@ -1146,18 +1147,6 @@
   </si>
   <si>
     <t>Speaker</t>
-  </si>
-  <si>
-    <t>2019 (#)</t>
-  </si>
-  <si>
-    <t>2019 (%)</t>
-  </si>
-  <si>
-    <t>2020 (#)</t>
-  </si>
-  <si>
-    <t>2020 (%)</t>
   </si>
   <si>
     <t>Number of attendees</t>
@@ -1303,12 +1292,65 @@
       <t>Unknown</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="7"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t>Reverse Book Club</t>
+    </r>
+  </si>
+  <si>
+    <t>Attendees 2019 (#)</t>
+  </si>
+  <si>
+    <t>Attendees 2019 (%)</t>
+  </si>
+  <si>
+    <t>Event Type 2019 (#)</t>
+  </si>
+  <si>
+    <t>Attendees 2020 (#)</t>
+  </si>
+  <si>
+    <t>Attendees 2020 (%)</t>
+  </si>
+  <si>
+    <t>Event Type 2020 (#)</t>
+  </si>
+  <si>
+    <t>Attendees per Event Type 2019 (#)</t>
+  </si>
+  <si>
+    <t>Attendees per Event Type 2020 (#)</t>
+  </si>
+  <si>
+    <t>Case Study</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="16">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1376,12 +1418,6 @@
       <name val="Graphik Meetup"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -1397,6 +1433,19 @@
       <sz val="7"/>
       <color rgb="FF000000"/>
       <name val="Times Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1487,11 +1536,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
@@ -1507,58 +1557,60 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="14" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1870,193 +1922,332 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{347026B8-9C3C-F240-8D3E-23690D0839F0}">
-  <dimension ref="D1:J11"/>
+  <dimension ref="B1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView zoomScale="119" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="4" max="4" width="35" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" customWidth="1"/>
+    <col min="2" max="2" width="35" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:10" ht="17" thickBot="1"/>
-    <row r="2" spans="4:10" ht="18" thickBot="1">
-      <c r="D2" s="15"/>
+    <row r="1" spans="2:10" ht="17" thickBot="1"/>
+    <row r="2" spans="2:10" ht="69" thickBot="1">
+      <c r="B2" s="15"/>
+      <c r="C2" s="16" t="s">
+        <v>381</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>382</v>
+      </c>
       <c r="E2" s="16" t="s">
+        <v>383</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>387</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>384</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>385</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>386</v>
+      </c>
+      <c r="J2" s="16" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10">
+      <c r="B3" s="27" t="s">
         <v>372</v>
       </c>
-      <c r="F2" s="16" t="s">
-        <v>373</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>374</v>
-      </c>
-      <c r="H2" s="16" t="s">
-        <v>375</v>
-      </c>
-      <c r="I2" s="17"/>
-      <c r="J2" s="18"/>
-    </row>
-    <row r="3" spans="4:10">
+      <c r="C3" s="25">
+        <v>83</v>
+      </c>
       <c r="D3" s="25" t="s">
-        <v>376</v>
-      </c>
-      <c r="E3" s="27">
-        <v>83</v>
-      </c>
-      <c r="F3" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="G3" s="27">
+      <c r="E3" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="G3" s="25">
         <v>113</v>
       </c>
       <c r="H3" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="I3" s="17"/>
-      <c r="J3" s="18"/>
-    </row>
-    <row r="4" spans="4:10" ht="17" thickBot="1">
+      <c r="I3" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="J3" s="25" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="17" thickBot="1">
+      <c r="B4" s="28"/>
+      <c r="C4" s="26"/>
       <c r="D4" s="26"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
       <c r="H4" s="30"/>
-      <c r="J4" s="18"/>
-    </row>
-    <row r="5" spans="4:10" ht="86" thickBot="1">
-      <c r="D5" s="19" t="s">
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+    </row>
+    <row r="5" spans="2:10" ht="35" thickBot="1">
+      <c r="B5" s="17" t="s">
+        <v>373</v>
+      </c>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+    </row>
+    <row r="6" spans="2:10" ht="18" thickBot="1">
+      <c r="B6" s="20" t="s">
+        <v>374</v>
+      </c>
+      <c r="C6" s="21">
+        <v>10</v>
+      </c>
+      <c r="D6" s="23">
+        <f>C6/SUM($C$6:$C$12)</f>
+        <v>0.12195121951219512</v>
+      </c>
+      <c r="E6" s="21">
+        <v>1</v>
+      </c>
+      <c r="F6" s="21">
+        <f>C6/E6</f>
+        <v>10</v>
+      </c>
+      <c r="G6" s="21">
+        <v>13</v>
+      </c>
+      <c r="H6" s="22">
+        <v>11.5</v>
+      </c>
+      <c r="I6" s="21">
+        <v>1</v>
+      </c>
+      <c r="J6" s="21">
+        <f>G6/I6</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" ht="18" thickBot="1">
+      <c r="B7" s="20" t="s">
+        <v>375</v>
+      </c>
+      <c r="C7" s="21">
+        <v>47</v>
+      </c>
+      <c r="D7" s="23">
+        <f t="shared" ref="D7" si="0">C7/SUM($C$6:$C$12)</f>
+        <v>0.57317073170731703</v>
+      </c>
+      <c r="E7" s="21">
+        <v>5</v>
+      </c>
+      <c r="F7" s="21">
+        <f>C7/E7</f>
+        <v>9.4</v>
+      </c>
+      <c r="G7" s="21">
+        <v>56</v>
+      </c>
+      <c r="H7" s="22">
+        <v>49.56</v>
+      </c>
+      <c r="I7" s="21">
+        <v>8</v>
+      </c>
+      <c r="J7" s="21">
+        <f>G7/I7</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" ht="18" thickBot="1">
+      <c r="B8" s="20" t="s">
+        <v>380</v>
+      </c>
+      <c r="C8" s="21">
+        <v>12</v>
+      </c>
+      <c r="D8" s="23">
+        <f>C8/SUM($C$6:$C$12)</f>
+        <v>0.14634146341463414</v>
+      </c>
+      <c r="E8" s="21">
+        <v>3</v>
+      </c>
+      <c r="F8" s="21">
+        <f t="shared" ref="F8:F12" si="1">C8/E8</f>
+        <v>4</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="H8" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="I8" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="J8" s="21" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" ht="18" thickBot="1">
+      <c r="B9" s="20" t="s">
+        <v>376</v>
+      </c>
+      <c r="C9" s="21">
+        <v>4</v>
+      </c>
+      <c r="D9" s="23">
+        <f>C9/SUM($C$6:$C$12)</f>
+        <v>4.878048780487805E-2</v>
+      </c>
+      <c r="E9" s="21">
+        <v>2</v>
+      </c>
+      <c r="F9" s="21">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="H9" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="I9" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="J9" s="21" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" ht="18" thickBot="1">
+      <c r="B10" s="20" t="s">
         <v>377</v>
       </c>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-    </row>
-    <row r="6" spans="4:10" ht="52" thickBot="1">
-      <c r="D6" s="22" t="s">
+      <c r="C10" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="G10" s="21">
+        <v>9</v>
+      </c>
+      <c r="H10" s="22">
+        <v>7.96</v>
+      </c>
+      <c r="I10" s="21">
+        <v>1</v>
+      </c>
+      <c r="J10" s="21">
+        <f t="shared" ref="J10:J12" si="2">G10/I10</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" ht="18" thickBot="1">
+      <c r="B11" s="20" t="s">
         <v>378</v>
       </c>
-      <c r="E6" s="23">
-        <v>10</v>
-      </c>
-      <c r="F6" s="23">
-        <v>12.05</v>
-      </c>
-      <c r="G6" s="23">
-        <v>13</v>
-      </c>
-      <c r="H6" s="24">
-        <v>11.5</v>
-      </c>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-    </row>
-    <row r="7" spans="4:10" ht="86" thickBot="1">
-      <c r="D7" s="22" t="s">
+      <c r="C11" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="G11" s="21">
+        <v>14</v>
+      </c>
+      <c r="H11" s="22">
+        <v>12.39</v>
+      </c>
+      <c r="I11" s="21">
+        <v>1</v>
+      </c>
+      <c r="J11" s="21">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" ht="18" thickBot="1">
+      <c r="B12" s="20" t="s">
         <v>379</v>
       </c>
-      <c r="E7" s="23">
-        <v>60</v>
-      </c>
-      <c r="F7" s="23">
-        <v>72.290000000000006</v>
-      </c>
-      <c r="G7" s="23">
-        <v>56</v>
-      </c>
-      <c r="H7" s="24">
-        <v>49.56</v>
-      </c>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-    </row>
-    <row r="8" spans="4:10" ht="69" thickBot="1">
-      <c r="D8" s="22" t="s">
-        <v>380</v>
-      </c>
-      <c r="E8" s="23">
+      <c r="C12" s="21">
+        <v>9</v>
+      </c>
+      <c r="D12" s="23">
+        <f>C12/SUM($C$6:$C$12)</f>
+        <v>0.10975609756097561</v>
+      </c>
+      <c r="E12" s="21">
+        <v>1</v>
+      </c>
+      <c r="F12" s="21">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="G12" s="21">
+        <v>0</v>
+      </c>
+      <c r="H12" s="22">
+        <v>0</v>
+      </c>
+      <c r="I12" s="21">
         <v>4</v>
       </c>
-      <c r="F8" s="23">
-        <v>4.82</v>
-      </c>
-      <c r="G8" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="H8" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-    </row>
-    <row r="9" spans="4:10" ht="52" thickBot="1">
-      <c r="D9" s="22" t="s">
-        <v>381</v>
-      </c>
-      <c r="E9" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="F9" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="G9" s="23">
-        <v>9</v>
-      </c>
-      <c r="H9" s="24">
-        <v>7.96</v>
-      </c>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-    </row>
-    <row r="10" spans="4:10" ht="69" thickBot="1">
-      <c r="D10" s="22" t="s">
-        <v>382</v>
-      </c>
-      <c r="E10" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="F10" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="G10" s="23">
-        <v>14</v>
-      </c>
-      <c r="H10" s="24">
-        <v>12.39</v>
-      </c>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-    </row>
-    <row r="11" spans="4:10" ht="69" thickBot="1">
-      <c r="D11" s="22" t="s">
-        <v>383</v>
-      </c>
-      <c r="E11" s="23">
-        <v>9</v>
-      </c>
-      <c r="F11" s="23">
-        <v>10.84</v>
-      </c>
-      <c r="G11" s="23">
+      <c r="J12" s="21">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H11" s="24">
-        <v>0</v>
-      </c>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
+    </row>
+    <row r="14" spans="2:10">
+      <c r="B14" s="24"/>
+    </row>
+    <row r="15" spans="2:10">
+      <c r="B15" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="D3:D4"/>
+  <mergeCells count="9">
+    <mergeCell ref="I3:I4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="H3:H4"/>
   </mergeCells>
@@ -2066,15 +2257,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E80064F0-1B5F-AB4F-B278-336F9B53E988}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:Z984"/>
   <sheetViews>
-    <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.5" customWidth="1"/>
     <col min="21" max="21" width="24.1640625" customWidth="1"/>
     <col min="22" max="22" width="24.33203125" customWidth="1"/>
   </cols>
@@ -2152,7 +2345,7 @@
       <c r="X1" s="3"/>
       <c r="Y1" s="3"/>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:26" hidden="1">
       <c r="A2" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -2192,7 +2385,7 @@
       <c r="Y2" s="3"/>
       <c r="Z2" s="3"/>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" hidden="1">
       <c r="A3" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -2232,7 +2425,7 @@
       <c r="Y3" s="3"/>
       <c r="Z3" s="3"/>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" hidden="1">
       <c r="A4" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -2272,7 +2465,7 @@
       <c r="Y4" s="3"/>
       <c r="Z4" s="3"/>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:26" hidden="1">
       <c r="A5" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -2312,7 +2505,7 @@
       <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:26" hidden="1">
       <c r="A6" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -2352,7 +2545,7 @@
       <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:26" hidden="1">
       <c r="A7" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -2392,7 +2585,7 @@
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:26" hidden="1">
       <c r="A8" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -2436,7 +2629,7 @@
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:26" hidden="1">
       <c r="A9" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -2476,7 +2669,7 @@
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
     </row>
-    <row r="10" spans="1:26">
+    <row r="10" spans="1:26" hidden="1">
       <c r="A10" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -2516,7 +2709,7 @@
       <c r="Y10" s="3"/>
       <c r="Z10" s="3"/>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:26" hidden="1">
       <c r="A11" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -2556,7 +2749,7 @@
       <c r="Y11" s="3"/>
       <c r="Z11" s="3"/>
     </row>
-    <row r="12" spans="1:26">
+    <row r="12" spans="1:26" hidden="1">
       <c r="A12" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -2596,7 +2789,7 @@
       <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:26" hidden="1">
       <c r="A13" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -2636,7 +2829,7 @@
       <c r="Y13" s="3"/>
       <c r="Z13" s="3"/>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:26" hidden="1">
       <c r="A14" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -2676,7 +2869,7 @@
       <c r="Y14" s="3"/>
       <c r="Z14" s="3"/>
     </row>
-    <row r="15" spans="1:26">
+    <row r="15" spans="1:26" hidden="1">
       <c r="A15" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -2716,7 +2909,7 @@
       <c r="Y15" s="3"/>
       <c r="Z15" s="3"/>
     </row>
-    <row r="16" spans="1:26">
+    <row r="16" spans="1:26" hidden="1">
       <c r="A16" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -2756,7 +2949,7 @@
       <c r="Y16" s="3"/>
       <c r="Z16" s="3"/>
     </row>
-    <row r="17" spans="1:26">
+    <row r="17" spans="1:26" hidden="1">
       <c r="A17" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -2796,7 +2989,7 @@
       <c r="Y17" s="3"/>
       <c r="Z17" s="3"/>
     </row>
-    <row r="18" spans="1:26">
+    <row r="18" spans="1:26" hidden="1">
       <c r="A18" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -2840,7 +3033,7 @@
       <c r="Y18" s="3"/>
       <c r="Z18" s="3"/>
     </row>
-    <row r="19" spans="1:26">
+    <row r="19" spans="1:26" hidden="1">
       <c r="A19" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -2880,7 +3073,7 @@
       <c r="Y19" s="3"/>
       <c r="Z19" s="3"/>
     </row>
-    <row r="20" spans="1:26">
+    <row r="20" spans="1:26" hidden="1">
       <c r="A20" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -2920,7 +3113,7 @@
       <c r="Y20" s="3"/>
       <c r="Z20" s="3"/>
     </row>
-    <row r="21" spans="1:26">
+    <row r="21" spans="1:26" hidden="1">
       <c r="A21" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -2960,7 +3153,7 @@
       <c r="Y21" s="3"/>
       <c r="Z21" s="3"/>
     </row>
-    <row r="22" spans="1:26">
+    <row r="22" spans="1:26" hidden="1">
       <c r="A22" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -3000,7 +3193,7 @@
       <c r="Y22" s="3"/>
       <c r="Z22" s="3"/>
     </row>
-    <row r="23" spans="1:26">
+    <row r="23" spans="1:26" hidden="1">
       <c r="A23" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -3040,7 +3233,7 @@
       <c r="Y23" s="3"/>
       <c r="Z23" s="3"/>
     </row>
-    <row r="24" spans="1:26">
+    <row r="24" spans="1:26" hidden="1">
       <c r="A24" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -3080,7 +3273,7 @@
       <c r="Y24" s="3"/>
       <c r="Z24" s="3"/>
     </row>
-    <row r="25" spans="1:26">
+    <row r="25" spans="1:26" hidden="1">
       <c r="A25" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -3120,7 +3313,7 @@
       <c r="Y25" s="3"/>
       <c r="Z25" s="3"/>
     </row>
-    <row r="26" spans="1:26">
+    <row r="26" spans="1:26" hidden="1">
       <c r="A26" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -3160,7 +3353,7 @@
       <c r="Y26" s="3"/>
       <c r="Z26" s="3"/>
     </row>
-    <row r="27" spans="1:26">
+    <row r="27" spans="1:26" hidden="1">
       <c r="A27" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -3204,7 +3397,7 @@
       <c r="Y27" s="3"/>
       <c r="Z27" s="3"/>
     </row>
-    <row r="28" spans="1:26">
+    <row r="28" spans="1:26" hidden="1">
       <c r="A28" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -3244,7 +3437,7 @@
       <c r="Y28" s="3"/>
       <c r="Z28" s="3"/>
     </row>
-    <row r="29" spans="1:26">
+    <row r="29" spans="1:26" hidden="1">
       <c r="A29" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -3284,7 +3477,7 @@
       <c r="Y29" s="3"/>
       <c r="Z29" s="3"/>
     </row>
-    <row r="30" spans="1:26">
+    <row r="30" spans="1:26" hidden="1">
       <c r="A30" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -3324,7 +3517,7 @@
       <c r="Y30" s="3"/>
       <c r="Z30" s="3"/>
     </row>
-    <row r="31" spans="1:26">
+    <row r="31" spans="1:26" hidden="1">
       <c r="A31" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -3364,7 +3557,7 @@
       <c r="Y31" s="3"/>
       <c r="Z31" s="3"/>
     </row>
-    <row r="32" spans="1:26">
+    <row r="32" spans="1:26" hidden="1">
       <c r="A32" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -3404,7 +3597,7 @@
       <c r="Y32" s="3"/>
       <c r="Z32" s="3"/>
     </row>
-    <row r="33" spans="1:26">
+    <row r="33" spans="1:26" hidden="1">
       <c r="A33" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -3444,7 +3637,7 @@
       <c r="Y33" s="3"/>
       <c r="Z33" s="3"/>
     </row>
-    <row r="34" spans="1:26">
+    <row r="34" spans="1:26" hidden="1">
       <c r="A34" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -3484,7 +3677,7 @@
       <c r="Y34" s="3"/>
       <c r="Z34" s="3"/>
     </row>
-    <row r="35" spans="1:26">
+    <row r="35" spans="1:26" hidden="1">
       <c r="A35" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -3522,7 +3715,7 @@
       <c r="Y35" s="3"/>
       <c r="Z35" s="3"/>
     </row>
-    <row r="36" spans="1:26">
+    <row r="36" spans="1:26" hidden="1">
       <c r="A36" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -3560,7 +3753,7 @@
       <c r="Y36" s="3"/>
       <c r="Z36" s="3"/>
     </row>
-    <row r="37" spans="1:26">
+    <row r="37" spans="1:26" hidden="1">
       <c r="A37" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -3598,7 +3791,7 @@
       <c r="Y37" s="3"/>
       <c r="Z37" s="3"/>
     </row>
-    <row r="38" spans="1:26">
+    <row r="38" spans="1:26" hidden="1">
       <c r="A38" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -3636,7 +3829,7 @@
       <c r="Y38" s="3"/>
       <c r="Z38" s="3"/>
     </row>
-    <row r="39" spans="1:26">
+    <row r="39" spans="1:26" hidden="1">
       <c r="A39" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -3674,7 +3867,7 @@
       <c r="Y39" s="3"/>
       <c r="Z39" s="3"/>
     </row>
-    <row r="40" spans="1:26">
+    <row r="40" spans="1:26" hidden="1">
       <c r="A40" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -3712,7 +3905,7 @@
       <c r="Y40" s="3"/>
       <c r="Z40" s="3"/>
     </row>
-    <row r="41" spans="1:26">
+    <row r="41" spans="1:26" hidden="1">
       <c r="A41" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -3750,7 +3943,7 @@
       <c r="Y41" s="3"/>
       <c r="Z41" s="3"/>
     </row>
-    <row r="42" spans="1:26">
+    <row r="42" spans="1:26" hidden="1">
       <c r="A42" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -3790,7 +3983,7 @@
       <c r="Y42" s="3"/>
       <c r="Z42" s="3"/>
     </row>
-    <row r="43" spans="1:26">
+    <row r="43" spans="1:26" hidden="1">
       <c r="A43" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -3830,7 +4023,7 @@
       <c r="Y43" s="3"/>
       <c r="Z43" s="3"/>
     </row>
-    <row r="44" spans="1:26">
+    <row r="44" spans="1:26" hidden="1">
       <c r="A44" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -3870,7 +4063,7 @@
       <c r="Y44" s="3"/>
       <c r="Z44" s="3"/>
     </row>
-    <row r="45" spans="1:26">
+    <row r="45" spans="1:26" hidden="1">
       <c r="A45" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -3910,7 +4103,7 @@
       <c r="Y45" s="3"/>
       <c r="Z45" s="3"/>
     </row>
-    <row r="46" spans="1:26">
+    <row r="46" spans="1:26" hidden="1">
       <c r="A46" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -3950,7 +4143,7 @@
       <c r="Y46" s="3"/>
       <c r="Z46" s="3"/>
     </row>
-    <row r="47" spans="1:26">
+    <row r="47" spans="1:26" hidden="1">
       <c r="A47" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -3990,7 +4183,7 @@
       <c r="Y47" s="3"/>
       <c r="Z47" s="3"/>
     </row>
-    <row r="48" spans="1:26">
+    <row r="48" spans="1:26" hidden="1">
       <c r="A48" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -4030,7 +4223,7 @@
       <c r="Y48" s="3"/>
       <c r="Z48" s="3"/>
     </row>
-    <row r="49" spans="1:26">
+    <row r="49" spans="1:26" hidden="1">
       <c r="A49" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -4070,7 +4263,7 @@
       <c r="Y49" s="3"/>
       <c r="Z49" s="3"/>
     </row>
-    <row r="50" spans="1:26">
+    <row r="50" spans="1:26" hidden="1">
       <c r="A50" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -4110,7 +4303,7 @@
       <c r="Y50" s="3"/>
       <c r="Z50" s="3"/>
     </row>
-    <row r="51" spans="1:26">
+    <row r="51" spans="1:26" hidden="1">
       <c r="A51" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -4150,7 +4343,7 @@
       <c r="Y51" s="3"/>
       <c r="Z51" s="3"/>
     </row>
-    <row r="52" spans="1:26">
+    <row r="52" spans="1:26" hidden="1">
       <c r="A52" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -4190,7 +4383,7 @@
       <c r="Y52" s="3"/>
       <c r="Z52" s="3"/>
     </row>
-    <row r="53" spans="1:26">
+    <row r="53" spans="1:26" hidden="1">
       <c r="A53" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -4228,7 +4421,7 @@
       <c r="Y53" s="3"/>
       <c r="Z53" s="3"/>
     </row>
-    <row r="54" spans="1:26">
+    <row r="54" spans="1:26" hidden="1">
       <c r="A54" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -4266,7 +4459,7 @@
       <c r="Y54" s="3"/>
       <c r="Z54" s="3"/>
     </row>
-    <row r="55" spans="1:26">
+    <row r="55" spans="1:26" hidden="1">
       <c r="A55" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -4304,7 +4497,7 @@
       <c r="Y55" s="3"/>
       <c r="Z55" s="3"/>
     </row>
-    <row r="56" spans="1:26">
+    <row r="56" spans="1:26" hidden="1">
       <c r="A56" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -4342,7 +4535,7 @@
       <c r="Y56" s="3"/>
       <c r="Z56" s="3"/>
     </row>
-    <row r="57" spans="1:26">
+    <row r="57" spans="1:26" hidden="1">
       <c r="A57" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -4380,7 +4573,7 @@
       <c r="Y57" s="3"/>
       <c r="Z57" s="3"/>
     </row>
-    <row r="58" spans="1:26">
+    <row r="58" spans="1:26" hidden="1">
       <c r="A58" s="6">
         <v>43788.177083333336</v>
       </c>
@@ -4418,7 +4611,7 @@
       <c r="Y58" s="3"/>
       <c r="Z58" s="3"/>
     </row>
-    <row r="59" spans="1:26">
+    <row r="59" spans="1:26" hidden="1">
       <c r="A59" s="6">
         <v>43738.308252314811</v>
       </c>
@@ -4472,7 +4665,7 @@
       <c r="Y59" s="3"/>
       <c r="Z59" s="3"/>
     </row>
-    <row r="60" spans="1:26">
+    <row r="60" spans="1:26" hidden="1">
       <c r="A60" s="6">
         <v>43738.558819444443</v>
       </c>
@@ -4524,7 +4717,7 @@
       <c r="Y60" s="3"/>
       <c r="Z60" s="3"/>
     </row>
-    <row r="61" spans="1:26">
+    <row r="61" spans="1:26" hidden="1">
       <c r="A61" s="6">
         <v>43738.755648148152</v>
       </c>
@@ -4574,7 +4767,7 @@
       <c r="Y61" s="3"/>
       <c r="Z61" s="3"/>
     </row>
-    <row r="62" spans="1:26">
+    <row r="62" spans="1:26" hidden="1">
       <c r="A62" s="6">
         <v>43738.771898148145</v>
       </c>
@@ -4624,7 +4817,7 @@
       <c r="Y62" s="3"/>
       <c r="Z62" s="3"/>
     </row>
-    <row r="63" spans="1:26">
+    <row r="63" spans="1:26" hidden="1">
       <c r="A63" s="6">
         <v>43738.773101851853</v>
       </c>
@@ -4674,7 +4867,7 @@
       <c r="Y63" s="3"/>
       <c r="Z63" s="3"/>
     </row>
-    <row r="64" spans="1:26">
+    <row r="64" spans="1:26" hidden="1">
       <c r="A64" s="6">
         <v>43738.774583333332</v>
       </c>
@@ -4724,7 +4917,7 @@
       <c r="Y64" s="3"/>
       <c r="Z64" s="3"/>
     </row>
-    <row r="65" spans="1:26">
+    <row r="65" spans="1:26" hidden="1">
       <c r="A65" s="6">
         <v>43738.777789351851</v>
       </c>
@@ -4778,7 +4971,7 @@
       <c r="Y65" s="3"/>
       <c r="Z65" s="3"/>
     </row>
-    <row r="66" spans="1:26">
+    <row r="66" spans="1:26" hidden="1">
       <c r="A66" s="6">
         <v>43738.780474537038</v>
       </c>
@@ -4828,7 +5021,7 @@
       <c r="Y66" s="3"/>
       <c r="Z66" s="3"/>
     </row>
-    <row r="67" spans="1:26">
+    <row r="67" spans="1:26" hidden="1">
       <c r="A67" s="6">
         <v>43738.784641203703</v>
       </c>
@@ -4882,7 +5075,7 @@
       <c r="Y67" s="3"/>
       <c r="Z67" s="3"/>
     </row>
-    <row r="68" spans="1:26">
+    <row r="68" spans="1:26" hidden="1">
       <c r="A68" s="6">
         <v>43738.869259259256</v>
       </c>
@@ -4932,7 +5125,7 @@
       <c r="Y68" s="3"/>
       <c r="Z68" s="3"/>
     </row>
-    <row r="69" spans="1:26">
+    <row r="69" spans="1:26" hidden="1">
       <c r="A69" s="6">
         <v>43738.870254629626</v>
       </c>
@@ -4982,7 +5175,7 @@
       <c r="Y69" s="3"/>
       <c r="Z69" s="3"/>
     </row>
-    <row r="70" spans="1:26">
+    <row r="70" spans="1:26" hidden="1">
       <c r="A70" s="6">
         <v>43745.82068287037</v>
       </c>
@@ -5036,7 +5229,7 @@
       <c r="Y70" s="3"/>
       <c r="Z70" s="3"/>
     </row>
-    <row r="71" spans="1:26">
+    <row r="71" spans="1:26" hidden="1">
       <c r="A71" s="6">
         <v>43747.232627314814</v>
       </c>
@@ -5086,7 +5279,7 @@
       <c r="Y71" s="3"/>
       <c r="Z71" s="3"/>
     </row>
-    <row r="72" spans="1:26">
+    <row r="72" spans="1:26" hidden="1">
       <c r="A72" s="6">
         <v>43766.768807870372</v>
       </c>
@@ -5132,7 +5325,7 @@
       <c r="Y72" s="3"/>
       <c r="Z72" s="3"/>
     </row>
-    <row r="73" spans="1:26">
+    <row r="73" spans="1:26" hidden="1">
       <c r="A73" s="6">
         <v>43766.778391203705</v>
       </c>
@@ -5194,7 +5387,7 @@
       <c r="Y73" s="3"/>
       <c r="Z73" s="3"/>
     </row>
-    <row r="74" spans="1:26">
+    <row r="74" spans="1:26" hidden="1">
       <c r="A74" s="6">
         <v>43766.779780092591</v>
       </c>
@@ -5248,7 +5441,7 @@
       <c r="Y74" s="3"/>
       <c r="Z74" s="3"/>
     </row>
-    <row r="75" spans="1:26">
+    <row r="75" spans="1:26" hidden="1">
       <c r="A75" s="6">
         <v>43766.771527777775</v>
       </c>
@@ -20096,6 +20289,11 @@
       <c r="M984" s="3"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:Z84" xr:uid="{A50171FF-3EB7-7E45-A84F-1006A6D46483}">
+    <filterColumn colId="20">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="mailto:annakirklandsmith@gmail.com" xr:uid="{38817229-7903-3145-9A49-9EA09C9000F5}"/>
     <hyperlink ref="D2" r:id="rId2" xr:uid="{1C3E9FE4-18A0-B74D-A607-BDA7FA22B87E}"/>
@@ -20221,16 +20419,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DC465E9-5747-FC42-803B-E43C9BB5FE73}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AA115"/>
   <sheetViews>
-    <sheetView topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="C107" sqref="C107"/>
+    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
+      <selection activeCell="C128" sqref="C128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="10.5" customWidth="1"/>
-    <col min="3" max="3" width="86.1640625" customWidth="1"/>
+    <col min="1" max="1" width="14.1640625" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="42.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27">
@@ -20307,7 +20507,8 @@
       <c r="Y1" s="3"/>
       <c r="Z1" s="3"/>
     </row>
-    <row r="3" spans="1:27">
+    <row r="2" spans="1:27" hidden="1"/>
+    <row r="3" spans="1:27" hidden="1">
       <c r="A3" s="6">
         <v>43857.760150462964</v>
       </c>
@@ -20356,7 +20557,7 @@
       <c r="Z3" s="3"/>
       <c r="AA3" s="3"/>
     </row>
-    <row r="4" spans="1:27">
+    <row r="4" spans="1:27" hidden="1">
       <c r="A4" s="6">
         <v>43857.763240740744</v>
       </c>
@@ -20407,7 +20608,7 @@
       <c r="Z4" s="3"/>
       <c r="AA4" s="3"/>
     </row>
-    <row r="5" spans="1:27">
+    <row r="5" spans="1:27" hidden="1">
       <c r="A5" s="6">
         <v>43857.765439814815</v>
       </c>
@@ -20452,7 +20653,7 @@
       <c r="Z5" s="3"/>
       <c r="AA5" s="3"/>
     </row>
-    <row r="6" spans="1:27">
+    <row r="6" spans="1:27" hidden="1">
       <c r="A6" s="6">
         <v>43857.767974537041</v>
       </c>
@@ -20501,7 +20702,7 @@
       <c r="Z6" s="3"/>
       <c r="AA6" s="3"/>
     </row>
-    <row r="7" spans="1:27">
+    <row r="7" spans="1:27" hidden="1">
       <c r="A7" s="6">
         <v>43857.773969907408</v>
       </c>
@@ -20552,7 +20753,7 @@
       <c r="Z7" s="3"/>
       <c r="AA7" s="3"/>
     </row>
-    <row r="8" spans="1:27">
+    <row r="8" spans="1:27" hidden="1">
       <c r="A8" s="6">
         <v>43857.775671296295</v>
       </c>
@@ -20603,7 +20804,7 @@
       <c r="Z8" s="3"/>
       <c r="AA8" s="3"/>
     </row>
-    <row r="9" spans="1:27">
+    <row r="9" spans="1:27" hidden="1">
       <c r="A9" s="6">
         <v>43857.776643518519</v>
       </c>
@@ -20652,7 +20853,7 @@
       <c r="Z9" s="3"/>
       <c r="AA9" s="3"/>
     </row>
-    <row r="10" spans="1:27">
+    <row r="10" spans="1:27" hidden="1">
       <c r="A10" s="6">
         <v>43857.848379629628</v>
       </c>
@@ -20701,7 +20902,7 @@
       <c r="Z10" s="3"/>
       <c r="AA10" s="3"/>
     </row>
-    <row r="11" spans="1:27">
+    <row r="11" spans="1:27" hidden="1">
       <c r="A11" s="5">
         <v>43857</v>
       </c>
@@ -20744,7 +20945,7 @@
       <c r="Z11" s="3"/>
       <c r="AA11" s="3"/>
     </row>
-    <row r="12" spans="1:27">
+    <row r="12" spans="1:27" hidden="1">
       <c r="A12" s="5">
         <v>43885</v>
       </c>
@@ -20813,7 +21014,7 @@
       <c r="Z12" s="3"/>
       <c r="AA12" s="3"/>
     </row>
-    <row r="13" spans="1:27">
+    <row r="13" spans="1:27" hidden="1">
       <c r="A13" s="6">
         <v>43885.392569444448</v>
       </c>
@@ -20864,7 +21065,7 @@
       <c r="Z13" s="3"/>
       <c r="AA13" s="3"/>
     </row>
-    <row r="14" spans="1:27">
+    <row r="14" spans="1:27" hidden="1">
       <c r="A14" s="6">
         <v>43885.532858796294</v>
       </c>
@@ -20923,7 +21124,7 @@
       <c r="Z14" s="3"/>
       <c r="AA14" s="3"/>
     </row>
-    <row r="15" spans="1:27">
+    <row r="15" spans="1:27" hidden="1">
       <c r="A15" s="6">
         <v>43885.65289351852</v>
       </c>
@@ -20972,7 +21173,7 @@
       <c r="Z15" s="3"/>
       <c r="AA15" s="3"/>
     </row>
-    <row r="16" spans="1:27">
+    <row r="16" spans="1:27" hidden="1">
       <c r="A16" s="6">
         <v>43885.720046296294</v>
       </c>
@@ -21039,7 +21240,7 @@
       <c r="Z16" s="3"/>
       <c r="AA16" s="3"/>
     </row>
-    <row r="17" spans="1:27">
+    <row r="17" spans="1:27" hidden="1">
       <c r="A17" s="6">
         <v>43885.72446759259</v>
       </c>
@@ -21088,7 +21289,7 @@
       <c r="Z17" s="3"/>
       <c r="AA17" s="3"/>
     </row>
-    <row r="18" spans="1:27">
+    <row r="18" spans="1:27" hidden="1">
       <c r="A18" s="6">
         <v>43885.742546296293</v>
       </c>
@@ -21137,7 +21338,7 @@
       <c r="Z18" s="3"/>
       <c r="AA18" s="3"/>
     </row>
-    <row r="19" spans="1:27">
+    <row r="19" spans="1:27" hidden="1">
       <c r="A19" s="6">
         <v>43885.758958333332</v>
       </c>
@@ -21204,7 +21405,7 @@
       <c r="Z19" s="3"/>
       <c r="AA19" s="3"/>
     </row>
-    <row r="20" spans="1:27">
+    <row r="20" spans="1:27" hidden="1">
       <c r="A20" s="6">
         <v>43885.765011574076</v>
       </c>
@@ -21255,7 +21456,7 @@
       <c r="Z20" s="3"/>
       <c r="AA20" s="3"/>
     </row>
-    <row r="21" spans="1:27">
+    <row r="21" spans="1:27" hidden="1">
       <c r="A21" s="6">
         <v>43885.766574074078</v>
       </c>
@@ -21304,7 +21505,7 @@
       <c r="Z21" s="3"/>
       <c r="AA21" s="3"/>
     </row>
-    <row r="22" spans="1:27">
+    <row r="22" spans="1:27" hidden="1">
       <c r="A22" s="6">
         <v>43885.770254629628</v>
       </c>
@@ -21353,7 +21554,7 @@
       <c r="Z22" s="3"/>
       <c r="AA22" s="3"/>
     </row>
-    <row r="23" spans="1:27">
+    <row r="23" spans="1:27" hidden="1">
       <c r="A23" s="6">
         <v>43885.847881944443</v>
       </c>
@@ -21400,7 +21601,7 @@
       <c r="Z23" s="3"/>
       <c r="AA23" s="3"/>
     </row>
-    <row r="24" spans="1:27">
+    <row r="24" spans="1:27" hidden="1">
       <c r="A24" s="6">
         <v>43885.84946759259</v>
       </c>
@@ -21445,7 +21646,7 @@
       <c r="Z24" s="3"/>
       <c r="AA24" s="3"/>
     </row>
-    <row r="25" spans="1:27">
+    <row r="25" spans="1:27" hidden="1">
       <c r="A25" s="6">
         <v>43885.851481481484</v>
       </c>
@@ -21496,7 +21697,7 @@
       <c r="Z25" s="3"/>
       <c r="AA25" s="3"/>
     </row>
-    <row r="26" spans="1:27">
+    <row r="26" spans="1:27" hidden="1">
       <c r="A26" s="6">
         <v>43885.853715277779</v>
       </c>
@@ -21541,7 +21742,7 @@
       <c r="Z26" s="3"/>
       <c r="AA26" s="3"/>
     </row>
-    <row r="27" spans="1:27">
+    <row r="27" spans="1:27" hidden="1">
       <c r="A27" s="6">
         <v>43920.37877314815</v>
       </c>
@@ -21592,7 +21793,7 @@
       <c r="Z27" s="3"/>
       <c r="AA27" s="3"/>
     </row>
-    <row r="28" spans="1:27">
+    <row r="28" spans="1:27" hidden="1">
       <c r="A28" s="6">
         <v>43920.439108796294</v>
       </c>
@@ -21641,7 +21842,7 @@
       <c r="Z28" s="3"/>
       <c r="AA28" s="3"/>
     </row>
-    <row r="29" spans="1:27">
+    <row r="29" spans="1:27" hidden="1">
       <c r="A29" s="7">
         <v>43920.603136574071</v>
       </c>
@@ -21706,7 +21907,7 @@
       <c r="Z29" s="3"/>
       <c r="AA29" s="3"/>
     </row>
-    <row r="30" spans="1:27">
+    <row r="30" spans="1:27" hidden="1">
       <c r="A30" s="7">
         <v>43920.446493055555</v>
       </c>
@@ -21755,7 +21956,7 @@
       <c r="Z30" s="3"/>
       <c r="AA30" s="3"/>
     </row>
-    <row r="31" spans="1:27">
+    <row r="31" spans="1:27" hidden="1">
       <c r="A31" s="6">
         <v>43920.765682870369</v>
       </c>
@@ -21806,7 +22007,7 @@
       <c r="Z31" s="3"/>
       <c r="AA31" s="3"/>
     </row>
-    <row r="32" spans="1:27">
+    <row r="32" spans="1:27" hidden="1">
       <c r="A32" s="6">
         <v>43920.7659375</v>
       </c>
@@ -21855,7 +22056,7 @@
       <c r="Z32" s="3"/>
       <c r="AA32" s="3"/>
     </row>
-    <row r="33" spans="1:27">
+    <row r="33" spans="1:27" hidden="1">
       <c r="A33" s="6">
         <v>43920.775821759256</v>
       </c>
@@ -21906,7 +22107,7 @@
       <c r="Z33" s="3"/>
       <c r="AA33" s="3"/>
     </row>
-    <row r="34" spans="1:27">
+    <row r="34" spans="1:27" hidden="1">
       <c r="A34" s="6">
         <v>43920.776886574073</v>
       </c>
@@ -21953,7 +22154,7 @@
       <c r="Z34" s="3"/>
       <c r="AA34" s="3"/>
     </row>
-    <row r="35" spans="1:27">
+    <row r="35" spans="1:27" hidden="1">
       <c r="A35" s="5">
         <v>43920</v>
       </c>
@@ -22002,7 +22203,7 @@
       <c r="Z35" s="3"/>
       <c r="AA35" s="3"/>
     </row>
-    <row r="36" spans="1:27">
+    <row r="36" spans="1:27" hidden="1">
       <c r="A36" s="5">
         <v>43920</v>
       </c>
@@ -22053,7 +22254,7 @@
       <c r="Z36" s="3"/>
       <c r="AA36" s="3"/>
     </row>
-    <row r="37" spans="1:27">
+    <row r="37" spans="1:27" hidden="1">
       <c r="A37" s="6">
         <v>43948.413159722222</v>
       </c>
@@ -22104,7 +22305,7 @@
       <c r="Z37" s="3"/>
       <c r="AA37" s="3"/>
     </row>
-    <row r="38" spans="1:27">
+    <row r="38" spans="1:27" hidden="1">
       <c r="A38" s="6">
         <v>43948.528078703705</v>
       </c>
@@ -22155,7 +22356,7 @@
       <c r="Z38" s="3"/>
       <c r="AA38" s="3"/>
     </row>
-    <row r="39" spans="1:27">
+    <row r="39" spans="1:27" hidden="1">
       <c r="A39" s="6">
         <v>43948.58630787037</v>
       </c>
@@ -22220,7 +22421,7 @@
       <c r="Z39" s="3"/>
       <c r="AA39" s="3"/>
     </row>
-    <row r="40" spans="1:27">
+    <row r="40" spans="1:27" hidden="1">
       <c r="A40" s="6">
         <v>43948.632002314815</v>
       </c>
@@ -22291,7 +22492,7 @@
       <c r="Z40" s="3"/>
       <c r="AA40" s="3"/>
     </row>
-    <row r="41" spans="1:27">
+    <row r="41" spans="1:27" hidden="1">
       <c r="A41" s="6">
         <v>43948.696932870371</v>
       </c>
@@ -22336,7 +22537,7 @@
       <c r="Z41" s="3"/>
       <c r="AA41" s="3"/>
     </row>
-    <row r="42" spans="1:27">
+    <row r="42" spans="1:27" hidden="1">
       <c r="A42" s="6">
         <v>43948.767314814817</v>
       </c>
@@ -22387,7 +22588,7 @@
       <c r="Z42" s="3"/>
       <c r="AA42" s="3"/>
     </row>
-    <row r="43" spans="1:27">
+    <row r="43" spans="1:27" hidden="1">
       <c r="A43" s="6">
         <v>43948.768692129626</v>
       </c>
@@ -22440,7 +22641,7 @@
       <c r="Z43" s="3"/>
       <c r="AA43" s="3"/>
     </row>
-    <row r="44" spans="1:27">
+    <row r="44" spans="1:27" hidden="1">
       <c r="A44" s="6">
         <v>43948.799675925926</v>
       </c>
@@ -22489,7 +22690,7 @@
       <c r="Z44" s="3"/>
       <c r="AA44" s="3"/>
     </row>
-    <row r="45" spans="1:27">
+    <row r="45" spans="1:27" hidden="1">
       <c r="A45" s="6">
         <v>43949.301388888889</v>
       </c>
@@ -22540,7 +22741,7 @@
       <c r="Z45" s="3"/>
       <c r="AA45" s="3"/>
     </row>
-    <row r="46" spans="1:27">
+    <row r="46" spans="1:27" hidden="1">
       <c r="A46" s="6">
         <v>43969.623981481483</v>
       </c>
@@ -22589,7 +22790,7 @@
       <c r="Z46" s="3"/>
       <c r="AA46" s="3"/>
     </row>
-    <row r="47" spans="1:27">
+    <row r="47" spans="1:27" hidden="1">
       <c r="A47" s="6">
         <v>43969.632916666669</v>
       </c>
@@ -22656,7 +22857,7 @@
       <c r="Z47" s="3"/>
       <c r="AA47" s="3"/>
     </row>
-    <row r="48" spans="1:27">
+    <row r="48" spans="1:27" hidden="1">
       <c r="A48" s="6">
         <v>43969.723055555558</v>
       </c>
@@ -22713,7 +22914,7 @@
       <c r="Z48" s="3"/>
       <c r="AA48" s="3"/>
     </row>
-    <row r="49" spans="1:27">
+    <row r="49" spans="1:27" hidden="1">
       <c r="A49" s="6">
         <v>43969.75271990741</v>
       </c>
@@ -22762,7 +22963,7 @@
       <c r="Z49" s="3"/>
       <c r="AA49" s="3"/>
     </row>
-    <row r="50" spans="1:27">
+    <row r="50" spans="1:27" hidden="1">
       <c r="A50" s="6">
         <v>43969.772453703707</v>
       </c>
@@ -22813,7 +23014,7 @@
       <c r="Z50" s="3"/>
       <c r="AA50" s="3"/>
     </row>
-    <row r="51" spans="1:27">
+    <row r="51" spans="1:27" hidden="1">
       <c r="A51" s="6">
         <v>43969.791307870371</v>
       </c>
@@ -22864,7 +23065,7 @@
       <c r="Z51" s="3"/>
       <c r="AA51" s="3"/>
     </row>
-    <row r="52" spans="1:27">
+    <row r="52" spans="1:27" hidden="1">
       <c r="A52" s="6">
         <v>43969.824699074074</v>
       </c>
@@ -22913,7 +23114,7 @@
       <c r="Z52" s="3"/>
       <c r="AA52" s="3"/>
     </row>
-    <row r="53" spans="1:27">
+    <row r="53" spans="1:27" hidden="1">
       <c r="A53" s="6">
         <v>44011.52140046296</v>
       </c>
@@ -22964,7 +23165,7 @@
       <c r="Z53" s="3"/>
       <c r="AA53" s="3"/>
     </row>
-    <row r="54" spans="1:27">
+    <row r="54" spans="1:27" hidden="1">
       <c r="A54" s="6">
         <v>44011.717638888891</v>
       </c>
@@ -23013,7 +23214,7 @@
       <c r="Z54" s="3"/>
       <c r="AA54" s="3"/>
     </row>
-    <row r="55" spans="1:27">
+    <row r="55" spans="1:27" hidden="1">
       <c r="A55" s="6">
         <v>44011.761562500003</v>
       </c>
@@ -23064,7 +23265,7 @@
       <c r="Z55" s="3"/>
       <c r="AA55" s="3"/>
     </row>
-    <row r="56" spans="1:27">
+    <row r="56" spans="1:27" hidden="1">
       <c r="A56" s="6">
         <v>44011.786458333336</v>
       </c>
@@ -23115,7 +23316,7 @@
       <c r="Z56" s="3"/>
       <c r="AA56" s="3"/>
     </row>
-    <row r="57" spans="1:27">
+    <row r="57" spans="1:27" hidden="1">
       <c r="A57" s="6">
         <v>44011.817627314813</v>
       </c>
@@ -23166,7 +23367,7 @@
       <c r="Z57" s="3"/>
       <c r="AA57" s="3"/>
     </row>
-    <row r="58" spans="1:27">
+    <row r="58" spans="1:27" hidden="1">
       <c r="A58" s="5">
         <v>44044</v>
       </c>
@@ -23231,7 +23432,7 @@
       <c r="Z58" s="3"/>
       <c r="AA58" s="3"/>
     </row>
-    <row r="59" spans="1:27">
+    <row r="59" spans="1:27" hidden="1">
       <c r="A59" s="5">
         <v>44044</v>
       </c>
@@ -23298,7 +23499,7 @@
       <c r="Z59" s="3"/>
       <c r="AA59" s="3"/>
     </row>
-    <row r="60" spans="1:27">
+    <row r="60" spans="1:27" hidden="1">
       <c r="A60" s="6">
         <v>44014.750787037039</v>
       </c>
@@ -23523,8 +23724,8 @@
       <c r="B64" s="5">
         <v>44020</v>
       </c>
-      <c r="C64" s="5" t="s">
-        <v>259</v>
+      <c r="C64" s="31" t="s">
+        <v>389</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>209</v>
@@ -23582,8 +23783,8 @@
       <c r="B65" s="5">
         <v>44020</v>
       </c>
-      <c r="C65" s="5" t="s">
-        <v>259</v>
+      <c r="C65" s="31" t="s">
+        <v>389</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>120</v>
@@ -23647,8 +23848,8 @@
       <c r="B66" s="5">
         <v>44020</v>
       </c>
-      <c r="C66" s="5" t="s">
-        <v>259</v>
+      <c r="C66" s="31" t="s">
+        <v>389</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>145</v>
@@ -23716,8 +23917,8 @@
       <c r="B67" s="5">
         <v>44020</v>
       </c>
-      <c r="C67" s="5" t="s">
-        <v>259</v>
+      <c r="C67" s="31" t="s">
+        <v>389</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>184</v>
@@ -23759,8 +23960,8 @@
       <c r="B68" s="5">
         <v>44020</v>
       </c>
-      <c r="C68" s="5" t="s">
-        <v>259</v>
+      <c r="C68" s="31" t="s">
+        <v>389</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>147</v>
@@ -23808,8 +24009,8 @@
       <c r="B69" s="5">
         <v>44020</v>
       </c>
-      <c r="C69" s="5" t="s">
-        <v>259</v>
+      <c r="C69" s="31" t="s">
+        <v>389</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>212</v>
@@ -23857,8 +24058,8 @@
       <c r="B70" s="5">
         <v>44020</v>
       </c>
-      <c r="C70" s="5" t="s">
-        <v>259</v>
+      <c r="C70" s="31" t="s">
+        <v>389</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>91</v>
@@ -23908,8 +24109,8 @@
       <c r="B71" s="5">
         <v>44020</v>
       </c>
-      <c r="C71" s="5" t="s">
-        <v>259</v>
+      <c r="C71" s="31" t="s">
+        <v>389</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>82</v>
@@ -23959,8 +24160,8 @@
       <c r="B72" s="5">
         <v>44020</v>
       </c>
-      <c r="C72" s="5" t="s">
-        <v>259</v>
+      <c r="C72" s="31" t="s">
+        <v>389</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>78</v>
@@ -24002,8 +24203,8 @@
       <c r="B73" s="5">
         <v>44020</v>
       </c>
-      <c r="C73" s="5" t="s">
-        <v>259</v>
+      <c r="C73" s="31" t="s">
+        <v>389</v>
       </c>
       <c r="D73" s="3"/>
       <c r="E73" s="2" t="s">
@@ -24036,7 +24237,7 @@
       <c r="Z73" s="3"/>
       <c r="AA73" s="3"/>
     </row>
-    <row r="74" spans="1:27">
+    <row r="74" spans="1:27" hidden="1">
       <c r="A74" s="6">
         <v>44039.750416666669</v>
       </c>
@@ -24089,7 +24290,7 @@
       <c r="Z74" s="3"/>
       <c r="AA74" s="3"/>
     </row>
-    <row r="75" spans="1:27">
+    <row r="75" spans="1:27" hidden="1">
       <c r="A75" s="6">
         <v>44039.848043981481</v>
       </c>
@@ -24138,7 +24339,7 @@
       <c r="Z75" s="3"/>
       <c r="AA75" s="3"/>
     </row>
-    <row r="76" spans="1:27">
+    <row r="76" spans="1:27" hidden="1">
       <c r="A76" s="6">
         <v>44039.863807870373</v>
       </c>
@@ -24183,7 +24384,7 @@
       <c r="Z76" s="3"/>
       <c r="AA76" s="3"/>
     </row>
-    <row r="77" spans="1:27">
+    <row r="77" spans="1:27" hidden="1">
       <c r="A77" s="6">
         <v>44074.673414351855</v>
       </c>
@@ -24234,7 +24435,7 @@
       <c r="Z77" s="3"/>
       <c r="AA77" s="3"/>
     </row>
-    <row r="78" spans="1:27">
+    <row r="78" spans="1:27" hidden="1">
       <c r="A78" s="6">
         <v>44074.767916666664</v>
       </c>
@@ -24283,7 +24484,7 @@
       <c r="Z78" s="3"/>
       <c r="AA78" s="3"/>
     </row>
-    <row r="79" spans="1:27">
+    <row r="79" spans="1:27" hidden="1">
       <c r="A79" s="6">
         <v>44074.771678240744</v>
       </c>
@@ -24330,7 +24531,7 @@
       <c r="Z79" s="3"/>
       <c r="AA79" s="3"/>
     </row>
-    <row r="80" spans="1:27">
+    <row r="80" spans="1:27" hidden="1">
       <c r="A80" s="6">
         <v>44074.776944444442</v>
       </c>
@@ -24375,7 +24576,7 @@
       <c r="Z80" s="3"/>
       <c r="AA80" s="3"/>
     </row>
-    <row r="81" spans="1:27">
+    <row r="81" spans="1:27" hidden="1">
       <c r="A81" s="6">
         <v>44074.777071759258</v>
       </c>
@@ -24420,7 +24621,7 @@
       <c r="Z81" s="3"/>
       <c r="AA81" s="3"/>
     </row>
-    <row r="82" spans="1:27">
+    <row r="82" spans="1:27" hidden="1">
       <c r="A82" s="6">
         <v>44074.797824074078</v>
       </c>
@@ -24469,7 +24670,7 @@
       <c r="Z82" s="3"/>
       <c r="AA82" s="3"/>
     </row>
-    <row r="83" spans="1:27">
+    <row r="83" spans="1:27" hidden="1">
       <c r="A83" s="6">
         <v>44074.832025462965</v>
       </c>
@@ -24538,7 +24739,7 @@
       <c r="Z83" s="3"/>
       <c r="AA83" s="3"/>
     </row>
-    <row r="84" spans="1:27">
+    <row r="84" spans="1:27" hidden="1">
       <c r="A84" s="6">
         <v>44074.844490740739</v>
       </c>
@@ -24589,7 +24790,7 @@
       <c r="Z84" s="3"/>
       <c r="AA84" s="3"/>
     </row>
-    <row r="85" spans="1:27">
+    <row r="85" spans="1:27" hidden="1">
       <c r="A85" s="6">
         <v>44076.76489583333</v>
       </c>
@@ -24640,7 +24841,7 @@
       <c r="Z85" s="3"/>
       <c r="AA85" s="3"/>
     </row>
-    <row r="86" spans="1:27">
+    <row r="86" spans="1:27" hidden="1">
       <c r="A86" s="6">
         <v>44082.881574074076</v>
       </c>
@@ -24693,7 +24894,7 @@
       <c r="Z86" s="3"/>
       <c r="AA86" s="3"/>
     </row>
-    <row r="87" spans="1:27">
+    <row r="87" spans="1:27" hidden="1">
       <c r="A87" s="6">
         <v>44102.748124999998</v>
       </c>
@@ -24742,7 +24943,7 @@
       <c r="Z87" s="3"/>
       <c r="AA87" s="3"/>
     </row>
-    <row r="88" spans="1:27">
+    <row r="88" spans="1:27" hidden="1">
       <c r="A88" s="6">
         <v>44102.768287037034</v>
       </c>
@@ -24811,7 +25012,7 @@
       <c r="Z88" s="3"/>
       <c r="AA88" s="3"/>
     </row>
-    <row r="89" spans="1:27">
+    <row r="89" spans="1:27" hidden="1">
       <c r="A89" s="6">
         <v>44102.771273148152</v>
       </c>
@@ -24858,7 +25059,7 @@
       <c r="Z89" s="3"/>
       <c r="AA89" s="3"/>
     </row>
-    <row r="90" spans="1:27">
+    <row r="90" spans="1:27" hidden="1">
       <c r="A90" s="6">
         <v>44102.772673611114</v>
       </c>
@@ -24907,7 +25108,7 @@
       <c r="Z90" s="3"/>
       <c r="AA90" s="3"/>
     </row>
-    <row r="91" spans="1:27">
+    <row r="91" spans="1:27" hidden="1">
       <c r="A91" s="6">
         <v>44102.772939814815</v>
       </c>
@@ -24956,7 +25157,7 @@
       <c r="Z91" s="3"/>
       <c r="AA91" s="3"/>
     </row>
-    <row r="92" spans="1:27">
+    <row r="92" spans="1:27" hidden="1">
       <c r="A92" s="6">
         <v>44102.773206018515</v>
       </c>
@@ -25005,7 +25206,7 @@
       <c r="Z92" s="3"/>
       <c r="AA92" s="3"/>
     </row>
-    <row r="93" spans="1:27">
+    <row r="93" spans="1:27" hidden="1">
       <c r="A93" s="6">
         <v>44102.778171296297</v>
       </c>
@@ -25052,7 +25253,7 @@
       <c r="Z93" s="3"/>
       <c r="AA93" s="3"/>
     </row>
-    <row r="94" spans="1:27">
+    <row r="94" spans="1:27" hidden="1">
       <c r="A94" s="6">
         <v>44102.812824074077</v>
       </c>
@@ -25113,7 +25314,7 @@
       <c r="Z94" s="3"/>
       <c r="AA94" s="3"/>
     </row>
-    <row r="95" spans="1:27">
+    <row r="95" spans="1:27" hidden="1">
       <c r="A95" s="5">
         <v>44044</v>
       </c>
@@ -25160,7 +25361,7 @@
       <c r="Z95" s="3"/>
       <c r="AA95" s="3"/>
     </row>
-    <row r="96" spans="1:27">
+    <row r="96" spans="1:27" hidden="1">
       <c r="A96" s="5">
         <v>44044</v>
       </c>
@@ -25201,7 +25402,7 @@
       <c r="Z96" s="3"/>
       <c r="AA96" s="3"/>
     </row>
-    <row r="97" spans="1:27">
+    <row r="97" spans="1:27" hidden="1">
       <c r="A97" s="5">
         <v>44044</v>
       </c>
@@ -25266,7 +25467,7 @@
       <c r="Z97" s="3"/>
       <c r="AA97" s="3"/>
     </row>
-    <row r="98" spans="1:27">
+    <row r="98" spans="1:27" hidden="1">
       <c r="A98" s="5">
         <v>43948</v>
       </c>
@@ -25313,7 +25514,7 @@
       <c r="Z98" s="3"/>
       <c r="AA98" s="3"/>
     </row>
-    <row r="99" spans="1:27">
+    <row r="99" spans="1:27" hidden="1">
       <c r="A99" s="5">
         <v>44082</v>
       </c>
@@ -25360,7 +25561,7 @@
       <c r="Z99" s="3"/>
       <c r="AA99" s="3"/>
     </row>
-    <row r="100" spans="1:27">
+    <row r="100" spans="1:27" hidden="1">
       <c r="A100" s="5">
         <v>44082</v>
       </c>
@@ -25409,7 +25610,7 @@
       <c r="Z100" s="3"/>
       <c r="AA100" s="3"/>
     </row>
-    <row r="101" spans="1:27">
+    <row r="101" spans="1:27" hidden="1">
       <c r="A101" s="5">
         <v>44082</v>
       </c>
@@ -25476,7 +25677,7 @@
       <c r="Z101" s="3"/>
       <c r="AA101" s="3"/>
     </row>
-    <row r="102" spans="1:27">
+    <row r="102" spans="1:27" hidden="1">
       <c r="A102" s="5">
         <v>44082</v>
       </c>
@@ -25525,7 +25726,7 @@
       <c r="Z102" s="3"/>
       <c r="AA102" s="3"/>
     </row>
-    <row r="103" spans="1:27">
+    <row r="103" spans="1:27" hidden="1">
       <c r="A103" s="5">
         <v>44082</v>
       </c>
@@ -25572,7 +25773,7 @@
       <c r="Z103" s="3"/>
       <c r="AA103" s="3"/>
     </row>
-    <row r="104" spans="1:27">
+    <row r="104" spans="1:27" hidden="1">
       <c r="A104" s="5">
         <v>44082</v>
       </c>
@@ -25613,7 +25814,7 @@
       <c r="Z104" s="3"/>
       <c r="AA104" s="3"/>
     </row>
-    <row r="105" spans="1:27">
+    <row r="105" spans="1:27" hidden="1">
       <c r="A105" s="5">
         <v>44082</v>
       </c>
@@ -25654,7 +25855,7 @@
       <c r="Z105" s="3"/>
       <c r="AA105" s="3"/>
     </row>
-    <row r="106" spans="1:27">
+    <row r="106" spans="1:27" hidden="1">
       <c r="A106" s="5">
         <v>44122</v>
       </c>
@@ -25695,7 +25896,7 @@
       <c r="Z106" s="3"/>
       <c r="AA106" s="3"/>
     </row>
-    <row r="107" spans="1:27">
+    <row r="107" spans="1:27" hidden="1">
       <c r="A107" s="5">
         <v>44122</v>
       </c>
@@ -25736,7 +25937,7 @@
       <c r="Z107" s="3"/>
       <c r="AA107" s="3"/>
     </row>
-    <row r="108" spans="1:27">
+    <row r="108" spans="1:27" hidden="1">
       <c r="A108" s="5">
         <v>44122</v>
       </c>
@@ -25783,7 +25984,7 @@
       <c r="Z108" s="3"/>
       <c r="AA108" s="3"/>
     </row>
-    <row r="109" spans="1:27">
+    <row r="109" spans="1:27" hidden="1">
       <c r="A109" s="5">
         <v>44122</v>
       </c>
@@ -25850,7 +26051,7 @@
       <c r="Z109" s="3"/>
       <c r="AA109" s="3"/>
     </row>
-    <row r="110" spans="1:27">
+    <row r="110" spans="1:27" hidden="1">
       <c r="A110" s="5">
         <v>44122</v>
       </c>
@@ -25915,7 +26116,7 @@
       <c r="Z110" s="3"/>
       <c r="AA110" s="3"/>
     </row>
-    <row r="111" spans="1:27">
+    <row r="111" spans="1:27" hidden="1">
       <c r="A111" s="5">
         <v>44122</v>
       </c>
@@ -25962,7 +26163,7 @@
       <c r="Z111" s="3"/>
       <c r="AA111" s="3"/>
     </row>
-    <row r="112" spans="1:27">
+    <row r="112" spans="1:27" hidden="1">
       <c r="A112" s="5">
         <v>44122</v>
       </c>
@@ -26011,7 +26212,7 @@
       <c r="Z112" s="3"/>
       <c r="AA112" s="3"/>
     </row>
-    <row r="113" spans="1:27">
+    <row r="113" spans="1:27" hidden="1">
       <c r="A113" s="5">
         <v>44122</v>
       </c>
@@ -26052,7 +26253,7 @@
       <c r="Z113" s="3"/>
       <c r="AA113" s="3"/>
     </row>
-    <row r="114" spans="1:27">
+    <row r="114" spans="1:27" hidden="1">
       <c r="A114" s="5">
         <v>44122</v>
       </c>
@@ -26119,7 +26320,7 @@
       <c r="Z114" s="3"/>
       <c r="AA114" s="3"/>
     </row>
-    <row r="115" spans="1:27">
+    <row r="115" spans="1:27" hidden="1">
       <c r="A115" s="5">
         <v>44122</v>
       </c>
@@ -26160,7 +26361,13 @@
       <c r="Z115" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="C1:C115" xr:uid="{FD262096-6DA5-124F-A638-FAF8E828BCB3}"/>
+  <autoFilter ref="C1:C115" xr:uid="{FD262096-6DA5-124F-A638-FAF8E828BCB3}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Project"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="E12" r:id="rId1" xr:uid="{F3088147-ED70-7F45-AFC6-5A41B42ED72D}"/>
     <hyperlink ref="E3" r:id="rId2" xr:uid="{149FA508-979D-7346-9F5C-945261AFFC72}"/>

</xml_diff>